<commit_message>
Increased notes field length to 2000 characters
</commit_message>
<xml_diff>
--- a/Customisations/Customisations.xlsx
+++ b/Customisations/Customisations.xlsx
@@ -437,7 +437,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -448,9 +448,6 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -488,7 +485,6 @@
     <col customWidth="1" min="3" max="3" width="13.43"/>
     <col customWidth="1" min="4" max="4" width="15.29"/>
     <col customWidth="1" min="5" max="21" width="4.71"/>
-    <col customWidth="1" min="22" max="26" width="12.57"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -2789,16 +2785,16 @@
       <c r="A26" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D26" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="E26" s="3" t="s">
         <v>96</v>
       </c>
       <c r="F26" s="2" t="b">
@@ -2813,11 +2809,9 @@
       <c r="I26" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J26" s="2">
-        <v>70.0</v>
-      </c>
-      <c r="K26" s="4">
-        <v>2000.0</v>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2">
+        <v>200.0</v>
       </c>
       <c r="L26" s="2" t="s">
         <v>35</v>
@@ -2825,8 +2819,8 @@
       <c r="M26" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="N26" s="2">
-        <v>200.0</v>
+      <c r="N26" s="4">
+        <v>2000.0</v>
       </c>
       <c r="O26" s="1" t="s">
         <v>36</v>
@@ -2991,7 +2985,6 @@
     <col customWidth="1" min="4" max="4" width="9.43"/>
     <col customWidth="1" min="5" max="5" width="21.14"/>
     <col customWidth="1" min="6" max="15" width="4.71"/>
-    <col customWidth="1" min="16" max="26" width="12.57"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -3247,10 +3240,10 @@
       <c r="C10" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="2">
         <v>5.0</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="2" t="s">
         <v>120</v>
       </c>
       <c r="F10" s="2"/>
@@ -19606,7 +19599,6 @@
     <col customWidth="1" min="4" max="4" width="18.43"/>
     <col customWidth="1" min="5" max="5" width="17.0"/>
     <col customWidth="1" min="6" max="21" width="4.71"/>
-    <col customWidth="1" min="22" max="26" width="12.57"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
Updated release package after adjusting form layouts
</commit_message>
<xml_diff>
--- a/Customisations/Customisations.xlsx
+++ b/Customisations/Customisations.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2330" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2330" uniqueCount="162">
   <si>
     <t>Display Name</t>
   </si>
@@ -506,6 +506,9 @@
   <si>
     <t>PM</t>
   </si>
+  <si>
+    <t>Only Run Between Hours Of</t>
+  </si>
 </sst>
 </file>
 
@@ -1477,7 +1480,7 @@
   <dimension ref="A1:Z36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3440,7 +3443,7 @@
         <v>132</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>133</v>
+        <v>161</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>50</v>

</xml_diff>

<commit_message>
Added a picklist for selecting the field to set when notification sent
</commit_message>
<xml_diff>
--- a/Customisations/Customisations.xlsx
+++ b/Customisations/Customisations.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2330" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2941" uniqueCount="165">
   <si>
     <t>Display Name</t>
   </si>
@@ -509,6 +509,15 @@
   <si>
     <t>Only Run Between Hours Of</t>
   </si>
+  <si>
+    <t>Set Field When Notification Sent Selection Field</t>
+  </si>
+  <si>
+    <t>Select to change the field to set</t>
+  </si>
+  <si>
+    <t>jmcg_setfieldwhennotificationsentselection</t>
+  </si>
 </sst>
 </file>
 
@@ -1477,10 +1486,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z36"/>
+  <dimension ref="A1:Z37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1489,7 +1498,7 @@
     <col min="2" max="2" width="54.7109375" customWidth="1"/>
     <col min="3" max="3" width="39.42578125" customWidth="1"/>
     <col min="4" max="4" width="9.140625" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" customWidth="1"/>
+    <col min="5" max="5" width="41.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.140625" customWidth="1"/>
     <col min="7" max="7" width="7.5703125" customWidth="1"/>
     <col min="8" max="8" width="4.7109375" customWidth="1"/>
@@ -3440,16 +3449,16 @@
         <v>12</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>132</v>
+        <v>164</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>133</v>
+        <v>162</v>
       </c>
       <c r="F30" s="2" t="b">
         <v>0</v>
@@ -3491,8 +3500,8 @@
       <c r="S30" s="1">
         <v>0</v>
       </c>
-      <c r="T30" s="1" t="s">
-        <v>46</v>
+      <c r="T30" s="5" t="s">
+        <v>162</v>
       </c>
       <c r="U30" s="2"/>
       <c r="V30" s="2"/>
@@ -3506,16 +3515,16 @@
         <v>12</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>62</v>
+        <v>161</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F31" s="2" t="b">
         <v>0</v>
@@ -3558,7 +3567,7 @@
         <v>0</v>
       </c>
       <c r="T31" s="1" t="s">
-        <v>146</v>
+        <v>46</v>
       </c>
       <c r="U31" s="2"/>
       <c r="V31" s="2"/>
@@ -3572,16 +3581,16 @@
         <v>12</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>62</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="F32" s="2" t="b">
         <v>0</v>
@@ -3624,7 +3633,7 @@
         <v>0</v>
       </c>
       <c r="T32" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="U32" s="2"/>
       <c r="V32" s="2"/>
@@ -3638,16 +3647,16 @@
         <v>12</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>62</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F33" s="2" t="b">
         <v>0</v>
@@ -3690,7 +3699,7 @@
         <v>0</v>
       </c>
       <c r="T33" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="U33" s="2"/>
       <c r="V33" s="2"/>
@@ -3704,16 +3713,16 @@
         <v>12</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>62</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F34" s="2" t="b">
         <v>0</v>
@@ -3756,7 +3765,7 @@
         <v>0</v>
       </c>
       <c r="T34" s="1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="U34" s="2"/>
       <c r="V34" s="2"/>
@@ -3770,16 +3779,16 @@
         <v>12</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>62</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F35" s="2" t="b">
         <v>0</v>
@@ -3822,7 +3831,7 @@
         <v>0</v>
       </c>
       <c r="T35" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="U35" s="2"/>
       <c r="V35" s="2"/>
@@ -3836,16 +3845,16 @@
         <v>12</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>62</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F36" s="2" t="b">
         <v>0</v>
@@ -3888,7 +3897,7 @@
         <v>0</v>
       </c>
       <c r="T36" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="U36" s="2"/>
       <c r="V36" s="2"/>
@@ -3897,12 +3906,78 @@
       <c r="Y36" s="2"/>
       <c r="Z36" s="2"/>
     </row>
+    <row r="37" spans="1:26" s="4" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="F37" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G37" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H37" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I37" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2">
+        <v>200</v>
+      </c>
+      <c r="L37" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="M37" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N37" s="4">
+        <v>2000</v>
+      </c>
+      <c r="O37" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P37" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q37" s="1">
+        <v>0</v>
+      </c>
+      <c r="R37" s="1">
+        <v>100000000</v>
+      </c>
+      <c r="S37" s="1">
+        <v>0</v>
+      </c>
+      <c r="T37" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="U37" s="2"/>
+      <c r="V37" s="2"/>
+      <c r="W37" s="2"/>
+      <c r="X37" s="2"/>
+      <c r="Y37" s="2"/>
+      <c r="Z37" s="2"/>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt=" - " sqref="O2:O1000">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt=" - " sqref="O2:O1001">
       <formula1>"Text,TextArea,Email,Url,TickerSymbol,Phone"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt=" - " sqref="D2:D30 D37:D1000">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt=" - " sqref="D38:D1001 D2:D31">
       <formula1>"Boolean,Date,Decimal,Double,Integer,Lookup,Money,Picklist,String,Memo,Status"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3912,16 +3987,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O689"/>
+  <dimension ref="A1:O889"/>
   <sheetViews>
-    <sheetView topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="D93" sqref="D93"/>
+    <sheetView topLeftCell="A861" workbookViewId="0">
+      <selection activeCell="B874" sqref="B874"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" customWidth="1"/>
+    <col min="1" max="1" width="44.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.140625" customWidth="1"/>
     <col min="4" max="4" width="9.42578125" customWidth="1"/>
     <col min="5" max="5" width="21.140625" style="8" customWidth="1"/>
@@ -22504,11 +22579,21 @@
       <c r="O688" s="2"/>
     </row>
     <row r="689" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A689" s="2"/>
-      <c r="B689" s="2"/>
-      <c r="C689" s="2"/>
-      <c r="D689" s="2"/>
-      <c r="E689" s="7"/>
+      <c r="A689" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B689" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C689" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D689" s="2">
+        <v>0</v>
+      </c>
+      <c r="E689" s="7" t="s">
+        <v>163</v>
+      </c>
       <c r="F689" s="2"/>
       <c r="G689" s="2"/>
       <c r="H689" s="2"/>
@@ -22519,6 +22604,3406 @@
       <c r="M689" s="2"/>
       <c r="N689" s="2"/>
       <c r="O689" s="2"/>
+    </row>
+    <row r="690" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A690" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B690" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C690" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D690" s="2">
+        <v>1</v>
+      </c>
+      <c r="E690" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="691" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A691" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B691" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C691" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D691" s="2">
+        <v>2</v>
+      </c>
+      <c r="E691" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="692" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A692" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B692" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C692" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D692" s="2">
+        <v>3</v>
+      </c>
+      <c r="E692" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="693" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A693" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B693" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C693" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D693" s="2">
+        <v>4</v>
+      </c>
+      <c r="E693" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="694" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A694" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B694" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C694" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D694" s="2">
+        <v>5</v>
+      </c>
+      <c r="E694" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="695" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A695" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B695" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C695" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D695" s="2">
+        <v>6</v>
+      </c>
+      <c r="E695" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="696" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A696" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B696" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C696" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D696" s="2">
+        <v>7</v>
+      </c>
+      <c r="E696" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="697" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A697" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B697" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C697" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D697" s="2">
+        <v>8</v>
+      </c>
+      <c r="E697" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="698" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A698" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B698" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C698" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D698" s="2">
+        <v>9</v>
+      </c>
+      <c r="E698" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="699" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A699" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B699" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C699" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D699" s="2">
+        <v>10</v>
+      </c>
+      <c r="E699" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="700" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A700" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B700" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C700" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D700" s="2">
+        <v>11</v>
+      </c>
+      <c r="E700" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="701" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A701" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B701" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C701" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D701" s="2">
+        <v>12</v>
+      </c>
+      <c r="E701" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="702" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A702" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B702" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C702" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D702" s="2">
+        <v>13</v>
+      </c>
+      <c r="E702" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="703" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A703" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B703" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C703" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D703" s="2">
+        <v>14</v>
+      </c>
+      <c r="E703" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="704" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A704" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B704" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C704" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D704" s="2">
+        <v>15</v>
+      </c>
+      <c r="E704" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="705" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A705" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B705" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C705" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D705" s="2">
+        <v>16</v>
+      </c>
+      <c r="E705" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="706" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A706" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B706" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C706" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D706" s="2">
+        <v>17</v>
+      </c>
+      <c r="E706" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="707" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A707" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B707" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C707" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D707" s="2">
+        <v>18</v>
+      </c>
+      <c r="E707" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="708" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A708" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B708" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C708" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D708" s="2">
+        <v>19</v>
+      </c>
+      <c r="E708" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="709" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A709" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B709" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C709" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D709" s="2">
+        <v>20</v>
+      </c>
+      <c r="E709" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="710" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A710" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B710" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C710" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D710" s="2">
+        <v>21</v>
+      </c>
+      <c r="E710" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="711" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A711" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B711" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C711" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D711" s="2">
+        <v>22</v>
+      </c>
+      <c r="E711" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="712" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A712" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B712" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C712" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D712" s="2">
+        <v>23</v>
+      </c>
+      <c r="E712" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="713" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A713" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B713" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C713" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D713" s="2">
+        <v>24</v>
+      </c>
+      <c r="E713" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="714" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A714" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B714" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C714" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D714" s="2">
+        <v>25</v>
+      </c>
+      <c r="E714" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="715" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A715" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B715" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C715" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D715" s="2">
+        <v>26</v>
+      </c>
+      <c r="E715" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="716" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A716" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B716" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C716" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D716" s="2">
+        <v>27</v>
+      </c>
+      <c r="E716" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="717" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A717" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B717" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C717" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D717" s="2">
+        <v>28</v>
+      </c>
+      <c r="E717" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="718" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A718" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B718" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C718" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D718" s="2">
+        <v>29</v>
+      </c>
+      <c r="E718" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="719" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A719" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B719" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C719" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D719" s="2">
+        <v>30</v>
+      </c>
+      <c r="E719" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="720" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A720" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B720" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C720" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D720" s="2">
+        <v>31</v>
+      </c>
+      <c r="E720" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="721" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A721" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B721" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C721" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D721" s="2">
+        <v>32</v>
+      </c>
+      <c r="E721" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="722" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A722" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B722" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C722" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D722" s="2">
+        <v>33</v>
+      </c>
+      <c r="E722" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="723" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A723" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B723" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C723" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D723" s="2">
+        <v>34</v>
+      </c>
+      <c r="E723" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="724" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A724" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B724" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C724" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D724" s="2">
+        <v>35</v>
+      </c>
+      <c r="E724" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="725" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A725" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B725" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C725" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D725" s="2">
+        <v>36</v>
+      </c>
+      <c r="E725" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="726" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A726" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B726" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C726" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D726" s="2">
+        <v>37</v>
+      </c>
+      <c r="E726" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="727" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A727" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B727" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C727" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D727" s="2">
+        <v>38</v>
+      </c>
+      <c r="E727" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="728" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A728" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B728" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C728" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D728" s="2">
+        <v>39</v>
+      </c>
+      <c r="E728" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="729" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A729" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B729" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C729" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D729" s="2">
+        <v>40</v>
+      </c>
+      <c r="E729" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="730" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A730" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B730" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C730" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D730" s="2">
+        <v>41</v>
+      </c>
+      <c r="E730" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="731" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A731" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B731" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C731" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D731" s="2">
+        <v>42</v>
+      </c>
+      <c r="E731" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="732" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A732" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B732" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C732" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D732" s="2">
+        <v>43</v>
+      </c>
+      <c r="E732" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="733" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A733" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B733" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C733" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D733" s="2">
+        <v>44</v>
+      </c>
+      <c r="E733" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="734" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A734" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B734" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C734" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D734" s="2">
+        <v>45</v>
+      </c>
+      <c r="E734" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="735" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A735" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B735" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C735" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D735" s="2">
+        <v>46</v>
+      </c>
+      <c r="E735" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="736" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A736" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B736" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C736" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D736" s="2">
+        <v>47</v>
+      </c>
+      <c r="E736" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="737" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A737" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B737" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C737" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D737" s="2">
+        <v>48</v>
+      </c>
+      <c r="E737" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="738" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A738" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B738" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C738" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D738" s="2">
+        <v>49</v>
+      </c>
+      <c r="E738" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="739" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A739" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B739" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C739" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D739" s="2">
+        <v>50</v>
+      </c>
+      <c r="E739" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="740" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A740" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B740" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C740" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D740" s="2">
+        <v>51</v>
+      </c>
+      <c r="E740" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="741" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A741" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B741" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C741" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D741" s="2">
+        <v>52</v>
+      </c>
+      <c r="E741" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="742" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A742" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B742" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C742" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D742" s="2">
+        <v>53</v>
+      </c>
+      <c r="E742" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="743" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A743" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B743" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C743" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D743" s="2">
+        <v>54</v>
+      </c>
+      <c r="E743" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="744" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A744" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B744" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C744" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D744" s="2">
+        <v>55</v>
+      </c>
+      <c r="E744" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="745" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A745" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B745" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C745" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D745" s="2">
+        <v>56</v>
+      </c>
+      <c r="E745" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="746" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A746" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B746" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C746" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D746" s="2">
+        <v>57</v>
+      </c>
+      <c r="E746" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="747" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A747" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B747" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C747" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D747" s="2">
+        <v>58</v>
+      </c>
+      <c r="E747" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="748" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A748" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B748" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C748" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D748" s="2">
+        <v>59</v>
+      </c>
+      <c r="E748" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="749" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A749" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B749" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C749" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D749" s="2">
+        <v>60</v>
+      </c>
+      <c r="E749" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="750" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A750" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B750" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C750" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D750" s="2">
+        <v>61</v>
+      </c>
+      <c r="E750" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="751" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A751" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B751" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C751" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D751" s="2">
+        <v>62</v>
+      </c>
+      <c r="E751" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="752" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A752" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B752" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C752" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D752" s="2">
+        <v>63</v>
+      </c>
+      <c r="E752" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="753" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A753" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B753" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C753" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D753" s="2">
+        <v>64</v>
+      </c>
+      <c r="E753" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="754" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A754" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B754" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C754" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D754" s="2">
+        <v>65</v>
+      </c>
+      <c r="E754" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="755" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A755" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B755" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C755" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D755" s="2">
+        <v>66</v>
+      </c>
+      <c r="E755" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="756" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A756" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B756" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C756" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D756" s="2">
+        <v>67</v>
+      </c>
+      <c r="E756" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="757" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A757" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B757" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C757" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D757" s="2">
+        <v>68</v>
+      </c>
+      <c r="E757" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="758" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A758" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B758" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C758" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D758" s="2">
+        <v>69</v>
+      </c>
+      <c r="E758" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="759" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A759" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B759" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C759" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D759" s="2">
+        <v>70</v>
+      </c>
+      <c r="E759" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="760" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A760" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B760" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C760" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D760" s="2">
+        <v>71</v>
+      </c>
+      <c r="E760" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="761" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A761" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B761" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C761" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D761" s="2">
+        <v>72</v>
+      </c>
+      <c r="E761" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="762" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A762" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B762" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C762" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D762" s="2">
+        <v>73</v>
+      </c>
+      <c r="E762" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="763" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A763" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B763" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C763" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D763" s="2">
+        <v>74</v>
+      </c>
+      <c r="E763" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="764" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A764" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B764" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C764" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D764" s="2">
+        <v>75</v>
+      </c>
+      <c r="E764" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="765" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A765" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B765" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C765" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D765" s="2">
+        <v>76</v>
+      </c>
+      <c r="E765" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="766" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A766" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B766" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C766" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D766" s="2">
+        <v>77</v>
+      </c>
+      <c r="E766" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="767" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A767" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B767" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C767" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D767" s="2">
+        <v>78</v>
+      </c>
+      <c r="E767" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="768" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A768" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B768" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C768" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D768" s="2">
+        <v>79</v>
+      </c>
+      <c r="E768" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="769" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A769" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B769" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C769" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D769" s="2">
+        <v>80</v>
+      </c>
+      <c r="E769" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="770" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A770" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B770" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C770" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D770" s="2">
+        <v>81</v>
+      </c>
+      <c r="E770" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="771" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A771" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B771" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C771" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D771" s="2">
+        <v>82</v>
+      </c>
+      <c r="E771" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="772" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A772" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B772" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C772" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D772" s="2">
+        <v>83</v>
+      </c>
+      <c r="E772" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="773" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A773" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B773" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C773" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D773" s="2">
+        <v>84</v>
+      </c>
+      <c r="E773" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="774" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A774" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B774" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C774" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D774" s="2">
+        <v>85</v>
+      </c>
+      <c r="E774" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="775" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A775" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B775" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C775" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D775" s="2">
+        <v>86</v>
+      </c>
+      <c r="E775" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="776" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A776" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B776" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C776" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D776" s="2">
+        <v>87</v>
+      </c>
+      <c r="E776" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="777" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A777" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B777" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C777" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D777" s="2">
+        <v>88</v>
+      </c>
+      <c r="E777" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="778" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A778" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B778" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C778" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D778" s="2">
+        <v>89</v>
+      </c>
+      <c r="E778" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="779" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A779" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B779" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C779" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D779" s="2">
+        <v>90</v>
+      </c>
+      <c r="E779" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="780" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A780" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B780" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C780" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D780" s="2">
+        <v>91</v>
+      </c>
+      <c r="E780" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="781" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A781" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B781" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C781" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D781" s="2">
+        <v>92</v>
+      </c>
+      <c r="E781" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="782" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A782" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B782" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C782" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D782" s="2">
+        <v>93</v>
+      </c>
+      <c r="E782" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="783" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A783" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B783" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C783" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D783" s="2">
+        <v>94</v>
+      </c>
+      <c r="E783" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="784" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A784" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B784" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C784" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D784" s="2">
+        <v>95</v>
+      </c>
+      <c r="E784" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="785" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A785" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B785" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C785" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D785" s="2">
+        <v>96</v>
+      </c>
+      <c r="E785" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="786" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A786" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B786" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C786" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D786" s="2">
+        <v>97</v>
+      </c>
+      <c r="E786" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="787" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A787" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B787" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C787" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D787" s="2">
+        <v>98</v>
+      </c>
+      <c r="E787" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="788" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A788" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B788" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C788" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D788" s="2">
+        <v>99</v>
+      </c>
+      <c r="E788" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="789" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A789" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B789" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C789" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D789" s="2">
+        <v>100</v>
+      </c>
+      <c r="E789" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="790" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A790" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B790" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C790" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D790" s="2">
+        <v>101</v>
+      </c>
+      <c r="E790" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="791" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A791" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B791" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C791" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D791" s="2">
+        <v>102</v>
+      </c>
+      <c r="E791" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="792" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A792" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B792" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C792" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D792" s="2">
+        <v>103</v>
+      </c>
+      <c r="E792" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="793" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A793" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B793" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C793" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D793" s="2">
+        <v>104</v>
+      </c>
+      <c r="E793" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="794" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A794" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B794" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C794" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D794" s="2">
+        <v>105</v>
+      </c>
+      <c r="E794" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="795" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A795" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B795" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C795" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D795" s="2">
+        <v>106</v>
+      </c>
+      <c r="E795" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="796" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A796" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B796" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C796" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D796" s="2">
+        <v>107</v>
+      </c>
+      <c r="E796" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="797" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A797" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B797" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C797" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D797" s="2">
+        <v>108</v>
+      </c>
+      <c r="E797" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="798" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A798" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B798" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C798" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D798" s="2">
+        <v>109</v>
+      </c>
+      <c r="E798" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="799" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A799" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B799" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C799" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D799" s="2">
+        <v>110</v>
+      </c>
+      <c r="E799" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="800" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A800" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B800" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C800" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D800" s="2">
+        <v>111</v>
+      </c>
+      <c r="E800" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="801" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A801" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B801" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C801" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D801" s="2">
+        <v>112</v>
+      </c>
+      <c r="E801" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="802" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A802" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B802" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C802" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D802" s="2">
+        <v>113</v>
+      </c>
+      <c r="E802" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="803" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A803" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B803" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C803" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D803" s="2">
+        <v>114</v>
+      </c>
+      <c r="E803" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="804" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A804" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B804" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C804" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D804" s="2">
+        <v>115</v>
+      </c>
+      <c r="E804" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="805" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A805" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B805" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C805" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D805" s="2">
+        <v>116</v>
+      </c>
+      <c r="E805" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="806" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A806" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B806" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C806" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D806" s="2">
+        <v>117</v>
+      </c>
+      <c r="E806" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="807" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A807" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B807" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C807" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D807" s="2">
+        <v>118</v>
+      </c>
+      <c r="E807" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="808" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A808" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B808" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C808" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D808" s="2">
+        <v>119</v>
+      </c>
+      <c r="E808" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="809" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A809" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B809" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C809" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D809" s="2">
+        <v>120</v>
+      </c>
+      <c r="E809" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="810" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A810" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B810" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C810" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D810" s="2">
+        <v>121</v>
+      </c>
+      <c r="E810" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="811" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A811" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B811" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C811" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D811" s="2">
+        <v>122</v>
+      </c>
+      <c r="E811" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="812" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A812" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B812" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C812" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D812" s="2">
+        <v>123</v>
+      </c>
+      <c r="E812" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="813" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A813" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B813" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C813" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D813" s="2">
+        <v>124</v>
+      </c>
+      <c r="E813" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="814" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A814" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B814" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C814" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D814" s="2">
+        <v>125</v>
+      </c>
+      <c r="E814" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="815" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A815" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B815" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C815" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D815" s="2">
+        <v>126</v>
+      </c>
+      <c r="E815" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="816" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A816" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B816" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C816" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D816" s="2">
+        <v>127</v>
+      </c>
+      <c r="E816" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="817" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A817" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B817" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C817" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D817" s="2">
+        <v>128</v>
+      </c>
+      <c r="E817" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="818" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A818" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B818" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C818" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D818" s="2">
+        <v>129</v>
+      </c>
+      <c r="E818" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="819" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A819" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B819" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C819" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D819" s="2">
+        <v>130</v>
+      </c>
+      <c r="E819" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="820" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A820" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B820" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C820" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D820" s="2">
+        <v>131</v>
+      </c>
+      <c r="E820" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="821" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A821" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B821" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C821" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D821" s="2">
+        <v>132</v>
+      </c>
+      <c r="E821" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="822" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A822" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B822" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C822" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D822" s="2">
+        <v>133</v>
+      </c>
+      <c r="E822" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="823" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A823" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B823" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C823" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D823" s="2">
+        <v>134</v>
+      </c>
+      <c r="E823" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="824" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A824" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B824" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C824" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D824" s="2">
+        <v>135</v>
+      </c>
+      <c r="E824" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="825" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A825" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B825" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C825" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D825" s="2">
+        <v>136</v>
+      </c>
+      <c r="E825" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="826" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A826" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B826" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C826" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D826" s="2">
+        <v>137</v>
+      </c>
+      <c r="E826" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="827" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A827" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B827" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C827" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D827" s="2">
+        <v>138</v>
+      </c>
+      <c r="E827" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="828" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A828" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B828" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C828" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D828" s="2">
+        <v>139</v>
+      </c>
+      <c r="E828" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="829" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A829" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B829" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C829" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D829" s="2">
+        <v>140</v>
+      </c>
+      <c r="E829" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="830" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A830" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B830" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C830" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D830" s="2">
+        <v>141</v>
+      </c>
+      <c r="E830" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="831" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A831" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B831" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C831" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D831" s="2">
+        <v>142</v>
+      </c>
+      <c r="E831" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="832" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A832" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B832" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C832" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D832" s="2">
+        <v>143</v>
+      </c>
+      <c r="E832" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="833" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A833" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B833" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C833" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D833" s="2">
+        <v>144</v>
+      </c>
+      <c r="E833" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="834" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A834" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B834" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C834" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D834" s="2">
+        <v>145</v>
+      </c>
+      <c r="E834" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="835" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A835" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B835" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C835" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D835" s="2">
+        <v>146</v>
+      </c>
+      <c r="E835" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="836" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A836" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B836" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C836" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D836" s="2">
+        <v>147</v>
+      </c>
+      <c r="E836" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="837" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A837" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B837" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C837" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D837" s="2">
+        <v>148</v>
+      </c>
+      <c r="E837" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="838" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A838" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B838" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C838" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D838" s="2">
+        <v>149</v>
+      </c>
+      <c r="E838" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="839" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A839" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B839" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C839" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D839" s="2">
+        <v>150</v>
+      </c>
+      <c r="E839" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="840" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A840" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B840" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C840" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D840" s="2">
+        <v>151</v>
+      </c>
+      <c r="E840" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="841" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A841" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B841" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C841" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D841" s="2">
+        <v>152</v>
+      </c>
+      <c r="E841" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="842" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A842" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B842" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C842" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D842" s="2">
+        <v>153</v>
+      </c>
+      <c r="E842" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="843" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A843" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B843" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C843" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D843" s="2">
+        <v>154</v>
+      </c>
+      <c r="E843" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="844" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A844" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B844" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C844" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D844" s="2">
+        <v>155</v>
+      </c>
+      <c r="E844" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="845" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A845" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B845" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C845" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D845" s="2">
+        <v>156</v>
+      </c>
+      <c r="E845" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="846" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A846" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B846" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C846" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D846" s="2">
+        <v>157</v>
+      </c>
+      <c r="E846" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="847" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A847" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B847" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C847" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D847" s="2">
+        <v>158</v>
+      </c>
+      <c r="E847" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="848" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A848" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B848" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C848" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D848" s="2">
+        <v>159</v>
+      </c>
+      <c r="E848" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="849" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A849" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B849" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C849" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D849" s="2">
+        <v>160</v>
+      </c>
+      <c r="E849" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="850" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A850" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B850" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C850" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D850" s="2">
+        <v>161</v>
+      </c>
+      <c r="E850" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="851" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A851" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B851" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C851" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D851" s="2">
+        <v>162</v>
+      </c>
+      <c r="E851" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="852" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A852" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B852" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C852" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D852" s="2">
+        <v>163</v>
+      </c>
+      <c r="E852" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="853" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A853" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B853" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C853" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D853" s="2">
+        <v>164</v>
+      </c>
+      <c r="E853" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="854" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A854" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B854" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C854" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D854" s="2">
+        <v>165</v>
+      </c>
+      <c r="E854" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="855" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A855" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B855" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C855" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D855" s="2">
+        <v>166</v>
+      </c>
+      <c r="E855" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="856" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A856" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B856" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C856" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D856" s="2">
+        <v>167</v>
+      </c>
+      <c r="E856" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="857" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A857" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B857" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C857" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D857" s="2">
+        <v>168</v>
+      </c>
+      <c r="E857" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="858" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A858" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B858" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C858" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D858" s="2">
+        <v>169</v>
+      </c>
+      <c r="E858" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="859" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A859" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B859" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C859" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D859" s="2">
+        <v>170</v>
+      </c>
+      <c r="E859" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="860" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A860" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B860" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C860" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D860" s="2">
+        <v>171</v>
+      </c>
+      <c r="E860" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="861" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A861" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B861" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C861" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D861" s="2">
+        <v>172</v>
+      </c>
+      <c r="E861" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="862" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A862" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B862" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C862" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D862" s="2">
+        <v>173</v>
+      </c>
+      <c r="E862" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="863" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A863" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B863" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C863" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D863" s="2">
+        <v>174</v>
+      </c>
+      <c r="E863" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="864" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A864" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B864" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C864" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D864" s="2">
+        <v>175</v>
+      </c>
+      <c r="E864" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="865" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A865" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B865" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C865" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D865" s="2">
+        <v>176</v>
+      </c>
+      <c r="E865" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="866" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A866" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B866" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C866" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D866" s="2">
+        <v>177</v>
+      </c>
+      <c r="E866" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="867" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A867" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B867" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C867" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D867" s="2">
+        <v>178</v>
+      </c>
+      <c r="E867" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="868" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A868" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B868" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C868" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D868" s="2">
+        <v>179</v>
+      </c>
+      <c r="E868" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="869" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A869" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B869" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C869" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D869" s="2">
+        <v>180</v>
+      </c>
+      <c r="E869" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="870" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A870" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B870" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C870" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D870" s="2">
+        <v>181</v>
+      </c>
+      <c r="E870" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="871" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A871" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B871" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C871" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D871" s="2">
+        <v>182</v>
+      </c>
+      <c r="E871" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="872" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A872" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B872" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C872" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D872" s="2">
+        <v>183</v>
+      </c>
+      <c r="E872" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="873" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A873" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B873" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C873" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D873" s="2">
+        <v>184</v>
+      </c>
+      <c r="E873" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="874" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A874" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B874" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C874" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D874" s="2">
+        <v>185</v>
+      </c>
+      <c r="E874" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="875" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A875" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B875" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C875" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D875" s="2">
+        <v>186</v>
+      </c>
+      <c r="E875" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="876" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A876" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B876" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C876" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D876" s="2">
+        <v>187</v>
+      </c>
+      <c r="E876" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="877" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A877" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B877" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C877" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D877" s="2">
+        <v>188</v>
+      </c>
+      <c r="E877" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="878" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A878" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B878" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C878" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D878" s="2">
+        <v>189</v>
+      </c>
+      <c r="E878" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="879" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A879" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B879" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C879" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D879" s="2">
+        <v>190</v>
+      </c>
+      <c r="E879" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="880" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A880" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B880" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C880" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D880" s="2">
+        <v>191</v>
+      </c>
+      <c r="E880" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="881" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A881" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B881" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C881" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D881" s="2">
+        <v>192</v>
+      </c>
+      <c r="E881" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="882" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A882" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B882" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C882" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D882" s="2">
+        <v>193</v>
+      </c>
+      <c r="E882" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="883" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A883" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B883" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C883" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D883" s="2">
+        <v>194</v>
+      </c>
+      <c r="E883" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="884" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A884" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B884" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C884" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D884" s="2">
+        <v>195</v>
+      </c>
+      <c r="E884" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="885" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A885" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B885" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C885" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D885" s="2">
+        <v>196</v>
+      </c>
+      <c r="E885" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="886" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A886" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B886" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C886" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D886" s="2">
+        <v>197</v>
+      </c>
+      <c r="E886" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="887" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A887" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B887" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C887" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D887" s="2">
+        <v>198</v>
+      </c>
+      <c r="E887" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="888" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A888" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B888" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C888" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D888" s="2">
+        <v>199</v>
+      </c>
+      <c r="E888" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="889" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A889" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B889" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C889" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D889" s="2">
+        <v>200</v>
+      </c>
+      <c r="E889" s="7" t="s">
+        <v>128</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added redundancy to the monitoring process
</commit_message>
<xml_diff>
--- a/Customisations/Customisations.xlsx
+++ b/Customisations/Customisations.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2941" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2957" uniqueCount="169">
   <si>
     <t>Display Name</t>
   </si>
@@ -518,6 +518,18 @@
   <si>
     <t>jmcg_setfieldwhennotificationsentselection</t>
   </si>
+  <si>
+    <t>jmcg_nextmonitortime</t>
+  </si>
+  <si>
+    <t>Next Monitor  Time</t>
+  </si>
+  <si>
+    <t>jmcg_nextmonitortime2</t>
+  </si>
+  <si>
+    <t>Next Monitor  Time 2</t>
+  </si>
 </sst>
 </file>
 
@@ -1486,10 +1498,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z37"/>
+  <dimension ref="A1:Z39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3972,12 +3984,148 @@
       <c r="Y37" s="2"/>
       <c r="Z37" s="2"/>
     </row>
+    <row r="38" spans="1:26" s="4" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F38" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G38" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H38" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I38" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J38" s="2">
+        <v>35</v>
+      </c>
+      <c r="K38" s="2">
+        <v>125</v>
+      </c>
+      <c r="L38" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="M38" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N38" s="2">
+        <v>200</v>
+      </c>
+      <c r="O38" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P38" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q38" s="1">
+        <v>0</v>
+      </c>
+      <c r="R38" s="1">
+        <v>100000000</v>
+      </c>
+      <c r="S38" s="1">
+        <v>0</v>
+      </c>
+      <c r="T38" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="U38" s="2"/>
+      <c r="V38" s="2"/>
+      <c r="W38" s="2"/>
+      <c r="X38" s="2"/>
+      <c r="Y38" s="2"/>
+      <c r="Z38" s="2"/>
+    </row>
+    <row r="39" spans="1:26" s="4" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="F39" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G39" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H39" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I39" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J39" s="2">
+        <v>35</v>
+      </c>
+      <c r="K39" s="2">
+        <v>125</v>
+      </c>
+      <c r="L39" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="M39" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N39" s="2">
+        <v>200</v>
+      </c>
+      <c r="O39" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P39" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q39" s="1">
+        <v>0</v>
+      </c>
+      <c r="R39" s="1">
+        <v>100000000</v>
+      </c>
+      <c r="S39" s="1">
+        <v>0</v>
+      </c>
+      <c r="T39" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="U39" s="2"/>
+      <c r="V39" s="2"/>
+      <c r="W39" s="2"/>
+      <c r="X39" s="2"/>
+      <c r="Y39" s="2"/>
+      <c r="Z39" s="2"/>
+    </row>
   </sheetData>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt=" - " sqref="O2:O1001">
       <formula1>"Text,TextArea,Email,Url,TickerSymbol,Phone"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt=" - " sqref="D38:D1001 D2:D31">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt=" - " sqref="D2:D31 D38:D1001">
       <formula1>"Boolean,Date,Decimal,Double,Integer,Lookup,Money,Picklist,String,Memo,Status"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>